<commit_message>
Randomizing The Excel File
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -271,17 +271,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,17 +287,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -316,24 +304,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,7 +610,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -638,7 +618,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -647,34 +627,34 @@
     </row>
     <row r="4" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -687,18 +667,18 @@
     </row>
     <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -710,19 +690,19 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
+      <c r="A12" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
+      <c r="A13" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -743,34 +723,34 @@
     </row>
     <row r="16" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,7 +770,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -798,59 +778,59 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>3</v>
+      <c r="A23" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,7 +850,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -887,74 +867,74 @@
     </row>
     <row r="34" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>12</v>
+      <c r="A42" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,26 +947,26 @@
     </row>
     <row r="44" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -999,58 +979,58 @@
     </row>
     <row r="48" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>12</v>
+      <c r="A52" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,18 +1043,18 @@
     </row>
     <row r="56" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1087,26 +1067,26 @@
     </row>
     <row r="59" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>